<commit_message>
read me and python path
</commit_message>
<xml_diff>
--- a/analysis/supplementary_materials/supplementary_spheroids_metrics.xlsx
+++ b/analysis/supplementary_materials/supplementary_spheroids_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lithic_Analysis\QSYSpheroidsStudy\analysis\supplementary_materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62435D0B-EF43-4D96-BD9B-F672AB9A6B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986673E7-4C0B-4B12-A8FC-03AB37ADD383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2ED60FBA-E623-4C3A-A256-DF261C5BABF6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="100">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -395,7 +395,6 @@
       <rPr>
         <sz val="12"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>平坦自然台面向对面剥片</t>
     </r>
@@ -447,7 +446,6 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -457,7 +455,6 @@
     <font>
       <sz val="10"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -474,7 +471,6 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -733,27 +729,36 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -768,15 +773,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1615,97 +1611,97 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22:Q22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1" spans="1:16" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="29" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="30"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="12" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="19" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="25"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:16" s="12" customFormat="1" ht="8.4" customHeight="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="13" t="s">
@@ -1891,7 +1887,7 @@
       <c r="M7" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="19" t="s">
         <v>99</v>
       </c>
       <c r="O7" s="14" t="s">
@@ -1938,7 +1934,7 @@
       <c r="M8" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="N8" s="19" t="s">
         <v>99</v>
       </c>
       <c r="O8" s="14" t="s">
@@ -2200,7 +2196,9 @@
         <v>32</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="H14" s="13">
         <v>14</v>
       </c>
@@ -2219,7 +2217,7 @@
       <c r="M14" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N14" s="33" t="s">
+      <c r="N14" s="19" t="s">
         <v>99</v>
       </c>
       <c r="O14" s="13" t="s">
@@ -2244,7 +2242,9 @@
         <v>92</v>
       </c>
       <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="H15" s="13" t="s">
         <v>96</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="M15" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N15" s="33" t="s">
+      <c r="N15" s="19" t="s">
         <v>99</v>
       </c>
       <c r="O15" s="13" t="s">
@@ -2309,7 +2309,7 @@
       <c r="M16" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="N16" s="33" t="s">
+      <c r="N16" s="19" t="s">
         <v>99</v>
       </c>
       <c r="O16" s="14" t="s">
@@ -2321,17 +2321,10 @@
       <c r="N17" s="13"/>
     </row>
     <row r="18" spans="14:14">
-      <c r="N18" s="33"/>
+      <c r="N18" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="N2:N3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:K1"/>
@@ -2341,6 +2334,13 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="14">

</xml_diff>